<commit_message>
mcu analogue pins doc added
</commit_message>
<xml_diff>
--- a/Pin Mappings.xlsx
+++ b/Pin Mappings.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\minec\Desktop\Work\GitHub Repos\PROJ515\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git\PROJ515\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD18ECBF-648C-4E51-AA16-1D71CDB346F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BDD4D390-9558-4E99-A693-EFE2BAB83CEC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{25789AAF-949D-45D3-BF4B-34A873866BAC}"/>
+    <workbookView xWindow="19200" yWindow="0" windowWidth="19200" windowHeight="21000" xr2:uid="{25789AAF-949D-45D3-BF4B-34A873866BAC}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -182,9 +182,6 @@
     <t>Light wake/sleep</t>
   </si>
   <si>
-    <t>mic_int1:mic_int0</t>
-  </si>
-  <si>
     <t>Acc_int</t>
   </si>
   <si>
@@ -200,9 +197,6 @@
     <t>PD15</t>
   </si>
   <si>
-    <t>PF12</t>
-  </si>
-  <si>
     <t>PF13</t>
   </si>
   <si>
@@ -291,6 +285,12 @@
   </si>
   <si>
     <t>PB2*</t>
+  </si>
+  <si>
+    <t>mic_int240:mic_int6k</t>
+  </si>
+  <si>
+    <t>PA6:Pf12</t>
   </si>
 </sst>
 </file>
@@ -3577,8 +3577,8 @@
       <xdr:row>36</xdr:row>
       <xdr:rowOff>80457</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId109">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="16" name="Ink 15">
@@ -3597,7 +3597,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="16" name="Ink 15">
@@ -5251,19 +5251,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E7554542-CFDC-4114-ADF7-E1610AA301DD}">
   <dimension ref="A1:D41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B35" sqref="B35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="23.140625" customWidth="1"/>
-    <col min="2" max="2" width="16.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="24.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.1796875" customWidth="1"/>
+    <col min="2" max="2" width="16.54296875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="24.1796875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.1796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="14" t="s">
         <v>0</v>
       </c>
@@ -5277,7 +5277,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" s="8" t="s">
         <v>2</v>
       </c>
@@ -5291,19 +5291,19 @@
         <v>17</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" s="3" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C3" s="5"/>
       <c r="D3" s="17" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" s="4" t="s">
         <v>7</v>
       </c>
@@ -5312,7 +5312,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5" s="3" t="s">
         <v>5</v>
       </c>
@@ -5324,7 +5324,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A6" s="3" t="s">
         <v>4</v>
       </c>
@@ -5336,7 +5336,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A7" s="3" t="s">
         <v>6</v>
       </c>
@@ -5348,7 +5348,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A8" s="3" t="s">
         <v>11</v>
       </c>
@@ -5362,7 +5362,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A9" s="8" t="s">
         <v>32</v>
       </c>
@@ -5374,16 +5374,16 @@
         <v>40</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A10" s="4" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B10" s="5"/>
       <c r="C10" s="5" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A11" s="3" t="s">
         <v>19</v>
       </c>
@@ -5391,50 +5391,50 @@
         <v>37</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="D11" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A12" s="3" t="s">
         <v>20</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="D12" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A13" s="8" t="s">
         <v>21</v>
       </c>
       <c r="B13" s="9" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C13" s="9" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="D13" s="10" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A14" s="4" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B14" s="5"/>
       <c r="C14" s="5" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A15" s="3" t="s">
         <v>22</v>
       </c>
@@ -5443,10 +5443,10 @@
       </c>
       <c r="C15" s="5"/>
       <c r="D15" s="11" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A16" s="3" t="s">
         <v>23</v>
       </c>
@@ -5455,10 +5455,10 @@
       </c>
       <c r="C16" s="5"/>
       <c r="D16" s="11" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A17" s="3" t="s">
         <v>24</v>
       </c>
@@ -5467,112 +5467,112 @@
       </c>
       <c r="C17" s="5"/>
       <c r="D17" s="11" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A18" s="3" t="s">
         <v>25</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C18" s="5"/>
       <c r="D18" s="11" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A19" s="8" t="s">
         <v>26</v>
       </c>
       <c r="B19" s="9" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C19" s="9"/>
       <c r="D19" s="10" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A20" s="4" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B20" s="5"/>
       <c r="C20" s="5"/>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A21" s="3" t="s">
         <v>22</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C21" s="5"/>
       <c r="D21" s="11" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A22" s="3" t="s">
         <v>23</v>
       </c>
       <c r="B22" s="5" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C22" s="5"/>
       <c r="D22" s="11" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A23" s="3" t="s">
         <v>24</v>
       </c>
       <c r="B23" s="5" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C23" s="5"/>
       <c r="D23" s="11" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A24" s="3" t="s">
         <v>25</v>
       </c>
       <c r="B24" s="5" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C24" s="5"/>
       <c r="D24" s="11" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A25" s="4" t="s">
         <v>31</v>
       </c>
       <c r="B25" s="5"/>
       <c r="C25" s="5"/>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A26" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="B26" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="C26" s="5" t="s">
         <v>68</v>
-      </c>
-      <c r="B26" s="5" t="s">
-        <v>69</v>
-      </c>
-      <c r="C26" s="5" t="s">
-        <v>70</v>
       </c>
       <c r="D26" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A27" s="8" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B27" s="9" t="s">
         <v>33</v>
@@ -5582,7 +5582,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A28" s="6" t="s">
         <v>41</v>
       </c>
@@ -5594,7 +5594,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A29" s="6" t="s">
         <v>43</v>
       </c>
@@ -5606,7 +5606,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A30" s="6" t="s">
         <v>44</v>
       </c>
@@ -5618,92 +5618,92 @@
         <v>17</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A31" s="8" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B31" s="9" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C31" s="9" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="D31" s="13" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A32" s="4" t="s">
         <v>45</v>
       </c>
       <c r="B32" s="5"/>
       <c r="C32" s="5"/>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A33" s="3" t="s">
         <v>46</v>
       </c>
       <c r="B33" s="5" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C33" s="5"/>
       <c r="D33" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A34" s="3" t="s">
         <v>47</v>
       </c>
       <c r="B34" s="5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C34" s="5"/>
       <c r="D34" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A35" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="B35" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="C35" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="D35" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A36" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="B35" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="C35" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="D35" t="s">
-        <v>59</v>
+      <c r="B36" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="C36" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="D36" t="s">
+        <v>57</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A36" s="3" t="s">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A37" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="B36" s="5" t="s">
-        <v>54</v>
-      </c>
-      <c r="C36" s="5" t="s">
-        <v>66</v>
-      </c>
-      <c r="D36" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A37" s="3" t="s">
-        <v>50</v>
-      </c>
       <c r="B37" s="5" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C37" s="5"/>
       <c r="D37" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A41" s="1" t="s">
         <v>39</v>
       </c>

</xml_diff>